<commit_message>
added the links and samples
</commit_message>
<xml_diff>
--- a/Vocabulary.xlsx
+++ b/Vocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Flask apps\Learn-French-with-Miti\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BC8C5C-3656-404D-814D-F21690544399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C0A56-913D-4C3C-9CB7-49A8E9C3FBF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22056" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="22056" windowHeight="13176" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wheather" sheetId="1" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>pantalon</t>
   </si>
   <si>
-    <t>petit-ami</t>
-  </si>
-  <si>
     <t>frère</t>
   </si>
   <si>
@@ -484,6 +481,9 @@
   </si>
   <si>
     <t>Tous les visiteurs sont priés de se présenter à la réception.</t>
+  </si>
+  <si>
+    <t>petit ami</t>
   </si>
 </sst>
 </file>
@@ -1960,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1972,7 +1972,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -1985,7 +1985,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2131,7 +2131,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2324,7 +2324,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2397,7 +2397,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2443,7 +2443,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -2455,7 +2455,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -2467,7 +2467,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2565,7 +2565,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2577,7 +2577,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -2590,7 +2590,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2603,7 +2603,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2616,7 +2616,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2629,7 +2629,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2642,7 +2642,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -2655,7 +2655,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2668,7 +2668,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2772,7 +2772,7 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2796,7 +2796,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -2809,7 +2809,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2823,7 +2823,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2836,7 +2836,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2849,7 +2849,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2863,7 +2863,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2877,7 +2877,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2891,7 +2891,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2904,7 +2904,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2918,7 +2918,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -2932,7 +2932,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -2946,7 +2946,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -2960,10 +2960,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E13" s="1"/>
     </row>
@@ -3090,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -3102,10 +3102,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -3117,7 +3117,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3128,7 +3128,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3140,7 +3140,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3152,7 +3152,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3176,7 +3176,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3188,7 +3188,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3200,7 +3200,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3212,7 +3212,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3224,7 +3224,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3236,10 +3236,10 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3282,7 +3282,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3294,10 +3294,10 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -3308,10 +3308,10 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -3323,10 +3323,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -3337,10 +3337,10 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -3352,10 +3352,10 @@
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -3367,10 +3367,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -3382,10 +3382,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -3395,10 +3395,10 @@
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -3409,10 +3409,10 @@
         <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -3424,10 +3424,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3439,7 +3439,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -3452,10 +3452,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3467,10 +3467,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3543,8 +3543,8 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -3567,7 +3567,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3579,20 +3579,20 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>IF(B3="la", "une",  IF(B3="le", "un", "not specified"))</f>
-        <v>not specified</v>
+        <v>un</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3603,7 +3603,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3615,7 +3615,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3627,7 +3627,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3669,7 +3669,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -3683,7 +3683,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -3692,10 +3692,10 @@
         <v>une-un</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -3704,13 +3704,13 @@
         <v>not specified</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -3719,10 +3719,10 @@
         <v>not specified</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -3825,7 +3825,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4006,7 +4006,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4053,7 +4053,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4077,7 +4077,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4133,7 +4133,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -4144,7 +4144,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -4155,7 +4155,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -4166,7 +4166,7 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -4178,7 +4178,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -4190,7 +4190,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -4202,10 +4202,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -4217,10 +4217,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -4232,10 +4232,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="42" x14ac:dyDescent="0.3">
@@ -4247,10 +4247,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -4376,7 +4376,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>